<commit_message>
Add Save to csv, character checking & some code cleanup
</commit_message>
<xml_diff>
--- a/TestFiles/TestBook.xlsx
+++ b/TestFiles/TestBook.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ExcelAddin4Magento\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\MagentoCsvExcelAddin\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,9 +25,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>This text was added by using code</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>TestB1</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>TestB2</t>
+  </si>
+  <si>
+    <t>TestB4</t>
+  </si>
+  <si>
+    <t>TestB5</t>
+  </si>
+  <si>
+    <t>TestB3</t>
   </si>
 </sst>
 </file>
@@ -378,15 +406,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>